<commit_message>
deja de prostituirte Ricardo Enrique Herrera Campos
</commit_message>
<xml_diff>
--- a/app/static/PDF/factura2_copia.xlsx
+++ b/app/static/PDF/factura2_copia.xlsx
@@ -905,7 +905,7 @@
     <outlinePr summaryBelow="0"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F63"/>
+  <dimension ref="A1:F62"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A5" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
       <selection activeCell="I12" sqref="I12"/>
@@ -962,7 +962,7 @@
       </c>
       <c r="F3" s="14" t="inlineStr">
         <is>
-          <t>F100-00000071</t>
+          <t>F100-00000087</t>
         </is>
       </c>
     </row>
@@ -1060,25 +1060,20 @@
     <row r="13" ht="19.5" customHeight="1">
       <c r="A13" s="51" t="inlineStr">
         <is>
-          <t>PANTALON 02 - cantidad: 1 - precio un.: S/. 78</t>
+          <t>PANTALON 04 - cantidad: 1 - precio un.: S/. 47</t>
         </is>
       </c>
       <c r="F13" s="51" t="n">
-        <v>78</v>
+        <v>47</v>
       </c>
     </row>
     <row r="14" ht="18.75" customHeight="1">
-      <c r="A14" s="51" t="inlineStr">
-        <is>
-          <t>PANTALON 03 - cantidad: 1 - precio un.: S/. 56</t>
-        </is>
-      </c>
-      <c r="F14" s="51" t="n">
-        <v>56</v>
-      </c>
+      <c r="A14" s="52" t="inlineStr"/>
+      <c r="E14" s="53" t="n"/>
+      <c r="F14" s="17" t="n"/>
     </row>
     <row r="15" ht="18.75" customHeight="1">
-      <c r="A15" s="52" t="inlineStr"/>
+      <c r="A15" s="54" t="n"/>
       <c r="E15" s="53" t="n"/>
       <c r="F15" s="17" t="n"/>
     </row>
@@ -1093,40 +1088,53 @@
       <c r="F17" s="17" t="n"/>
     </row>
     <row r="18" ht="18.75" customHeight="1">
-      <c r="A18" s="54" t="n"/>
-      <c r="E18" s="53" t="n"/>
-      <c r="F18" s="17" t="n"/>
+      <c r="A18" s="55" t="n"/>
+      <c r="B18" s="56" t="n"/>
+      <c r="C18" s="56" t="n"/>
+      <c r="D18" s="56" t="n"/>
+      <c r="E18" s="57" t="n"/>
+      <c r="F18" s="18" t="n"/>
     </row>
     <row r="19" ht="18.75" customHeight="1">
-      <c r="A19" s="55" t="n"/>
-      <c r="B19" s="56" t="n"/>
-      <c r="C19" s="56" t="n"/>
-      <c r="D19" s="56" t="n"/>
-      <c r="E19" s="57" t="n"/>
-      <c r="F19" s="18" t="n"/>
+      <c r="A19" s="39" t="n"/>
+      <c r="B19" s="58" t="n"/>
+      <c r="C19" s="58" t="n"/>
+      <c r="D19" s="21" t="inlineStr">
+        <is>
+          <t>[42]</t>
+        </is>
+      </c>
+      <c r="E19" s="19" t="inlineStr">
+        <is>
+          <t>SUBTOTAL</t>
+        </is>
+      </c>
+      <c r="F19" s="4" t="n">
+        <v>47</v>
+      </c>
     </row>
     <row r="20" ht="18.75" customHeight="1">
-      <c r="A20" s="39" t="n"/>
+      <c r="A20" s="38" t="inlineStr">
+        <is>
+          <t>COMENTARIOS</t>
+        </is>
+      </c>
       <c r="B20" s="58" t="n"/>
-      <c r="C20" s="58" t="n"/>
-      <c r="D20" s="21" t="inlineStr">
-        <is>
-          <t>[42]</t>
-        </is>
-      </c>
+      <c r="C20" s="59" t="n"/>
+      <c r="D20" s="43" t="n"/>
       <c r="E20" s="19" t="inlineStr">
         <is>
-          <t>SUBTOTAL</t>
-        </is>
-      </c>
-      <c r="F20" s="4" t="n">
-        <v>134</v>
+          <t>TASA DE IMPUESTO</t>
+        </is>
+      </c>
+      <c r="F20" s="20" t="n">
+        <v>18</v>
       </c>
     </row>
     <row r="21" ht="18.75" customHeight="1" thickBot="1">
-      <c r="A21" s="38" t="inlineStr">
-        <is>
-          <t>COMENTARIOS</t>
+      <c r="A21" s="30" t="inlineStr">
+        <is>
+          <t>1. Total a pagar en 30 días</t>
         </is>
       </c>
       <c r="B21" s="58" t="n"/>
@@ -1134,72 +1142,62 @@
       <c r="D21" s="43" t="n"/>
       <c r="E21" s="19" t="inlineStr">
         <is>
-          <t>TASA DE IMPUESTO</t>
-        </is>
-      </c>
-      <c r="F21" s="20" t="n">
-        <v>18</v>
+          <t>IMPUESTO</t>
+        </is>
+      </c>
+      <c r="F21" s="4" t="n">
+        <v>8.460000000000001</v>
       </c>
     </row>
     <row r="22" ht="18.75" customHeight="1">
       <c r="A22" s="30" t="inlineStr">
         <is>
-          <t>1. Total a pagar en 30 días</t>
+          <t>2. Incluya por favor el número de factura en su cheque</t>
         </is>
       </c>
       <c r="B22" s="58" t="n"/>
       <c r="C22" s="59" t="n"/>
       <c r="D22" s="43" t="n"/>
-      <c r="E22" s="19" t="inlineStr">
-        <is>
-          <t>IMPUESTO</t>
-        </is>
-      </c>
-      <c r="F22" s="4" t="n">
-        <v>24.12</v>
+      <c r="E22" s="24" t="inlineStr">
+        <is>
+          <t>OTRO</t>
+        </is>
+      </c>
+      <c r="F22" s="25" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
       </c>
     </row>
     <row r="23" ht="18.75" customHeight="1">
-      <c r="A23" s="30" t="inlineStr">
-        <is>
-          <t>2. Incluya por favor el número de factura en su cheque</t>
-        </is>
-      </c>
-      <c r="B23" s="58" t="n"/>
-      <c r="C23" s="59" t="n"/>
+      <c r="A23" s="27" t="n"/>
+      <c r="B23" s="27" t="n"/>
+      <c r="C23" s="27" t="n"/>
       <c r="D23" s="43" t="n"/>
-      <c r="E23" s="24" t="inlineStr">
-        <is>
-          <t>OTRO</t>
-        </is>
-      </c>
-      <c r="F23" s="25" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
+      <c r="E23" s="22" t="inlineStr">
+        <is>
+          <t>TOTAL</t>
+        </is>
+      </c>
+      <c r="F23" s="23" t="n">
+        <v>55.46</v>
       </c>
     </row>
     <row r="24" ht="18.75" customHeight="1">
       <c r="A24" s="27" t="n"/>
       <c r="B24" s="27" t="n"/>
       <c r="C24" s="27" t="n"/>
-      <c r="D24" s="43" t="n"/>
-      <c r="E24" s="22" t="inlineStr">
-        <is>
-          <t>TOTAL</t>
-        </is>
-      </c>
-      <c r="F24" s="23" t="n">
-        <v>158.12</v>
-      </c>
+      <c r="D24" s="6" t="n"/>
+      <c r="E24" s="6" t="n"/>
+      <c r="F24" s="5" t="n"/>
     </row>
     <row r="25" ht="18.75" customHeight="1">
       <c r="A25" s="27" t="n"/>
       <c r="B25" s="27" t="n"/>
       <c r="C25" s="27" t="n"/>
-      <c r="D25" s="6" t="n"/>
-      <c r="E25" s="6" t="n"/>
-      <c r="F25" s="5" t="n"/>
+      <c r="D25" s="27" t="n"/>
+      <c r="E25" s="27" t="n"/>
+      <c r="F25" s="27" t="n"/>
     </row>
     <row r="26" ht="18.75" customHeight="1">
       <c r="A26" s="27" t="n"/>
@@ -1213,41 +1211,41 @@
       <c r="A27" s="27" t="n"/>
       <c r="B27" s="27" t="n"/>
       <c r="C27" s="27" t="n"/>
-      <c r="D27" s="27" t="n"/>
-      <c r="E27" s="27" t="n"/>
-      <c r="F27" s="27" t="n"/>
+      <c r="D27" s="28" t="n"/>
+      <c r="E27" s="28" t="n"/>
+      <c r="F27" s="29" t="n"/>
     </row>
     <row r="28" ht="18.75" customHeight="1">
       <c r="A28" s="27" t="n"/>
       <c r="B28" s="27" t="n"/>
       <c r="C28" s="27" t="n"/>
-      <c r="D28" s="28" t="n"/>
-      <c r="E28" s="28" t="n"/>
-      <c r="F28" s="29" t="n"/>
+      <c r="D28" s="27" t="n"/>
+      <c r="E28" s="27" t="n"/>
+      <c r="F28" s="27" t="n"/>
     </row>
     <row r="29" ht="19.5" customHeight="1">
       <c r="A29" s="27" t="n"/>
       <c r="B29" s="27" t="n"/>
       <c r="C29" s="27" t="n"/>
-      <c r="D29" s="27" t="n"/>
-      <c r="E29" s="27" t="n"/>
-      <c r="F29" s="27" t="n"/>
+      <c r="D29" s="43" t="n"/>
+      <c r="E29" s="43" t="n"/>
+      <c r="F29" s="5" t="n"/>
     </row>
     <row r="30">
       <c r="A30" s="27" t="n"/>
       <c r="B30" s="27" t="n"/>
       <c r="C30" s="27" t="n"/>
-      <c r="D30" s="43" t="n"/>
-      <c r="E30" s="43" t="n"/>
-      <c r="F30" s="5" t="n"/>
+      <c r="D30" s="28" t="n"/>
+      <c r="E30" s="28" t="n"/>
+      <c r="F30" s="29" t="n"/>
     </row>
     <row r="31">
       <c r="A31" s="27" t="n"/>
       <c r="B31" s="27" t="n"/>
       <c r="C31" s="27" t="n"/>
-      <c r="D31" s="28" t="n"/>
-      <c r="E31" s="28" t="n"/>
-      <c r="F31" s="29" t="n"/>
+      <c r="D31" s="6" t="n"/>
+      <c r="E31" s="6" t="n"/>
+      <c r="F31" s="26" t="n"/>
     </row>
     <row r="32">
       <c r="A32" s="27" t="n"/>
@@ -1261,9 +1259,6 @@
       <c r="A33" s="27" t="n"/>
       <c r="B33" s="27" t="n"/>
       <c r="C33" s="27" t="n"/>
-      <c r="D33" s="6" t="n"/>
-      <c r="E33" s="6" t="n"/>
-      <c r="F33" s="26" t="n"/>
     </row>
     <row r="34">
       <c r="A34" s="27" t="n"/>
@@ -1409,11 +1404,6 @@
       <c r="A62" s="27" t="n"/>
       <c r="B62" s="27" t="n"/>
       <c r="C62" s="27" t="n"/>
-    </row>
-    <row r="63">
-      <c r="A63" s="27" t="n"/>
-      <c r="B63" s="27" t="n"/>
-      <c r="C63" s="27" t="n"/>
     </row>
   </sheetData>
   <mergeCells count="13">

</xml_diff>

<commit_message>
Vayanse todos a la mierda
</commit_message>
<xml_diff>
--- a/app/static/PDF/factura2_copia.xlsx
+++ b/app/static/PDF/factura2_copia.xlsx
@@ -905,7 +905,7 @@
     <outlinePr summaryBelow="0"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F62"/>
+  <dimension ref="A1:F64"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A5" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
       <selection activeCell="I12" sqref="I12"/>
@@ -946,7 +946,7 @@
       </c>
       <c r="F2" s="12" t="inlineStr">
         <is>
-          <t>2024-11-03</t>
+          <t>2024-11-05</t>
         </is>
       </c>
     </row>
@@ -962,7 +962,7 @@
       </c>
       <c r="F3" s="14" t="inlineStr">
         <is>
-          <t>F100-00000087</t>
+          <t>F100-00000013</t>
         </is>
       </c>
     </row>
@@ -1060,25 +1060,35 @@
     <row r="13" ht="19.5" customHeight="1">
       <c r="A13" s="51" t="inlineStr">
         <is>
+          <t>PANTALON 06 - cantidad: 1 - precio un.: S/. 69</t>
+        </is>
+      </c>
+      <c r="F13" s="51" t="n">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="14" ht="18.75" customHeight="1">
+      <c r="A14" s="51" t="inlineStr">
+        <is>
+          <t>PANTALON 05 - cantidad: 1 - precio un.: S/. 57</t>
+        </is>
+      </c>
+      <c r="F14" s="51" t="n">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="15" ht="18.75" customHeight="1">
+      <c r="A15" s="51" t="inlineStr">
+        <is>
           <t>PANTALON 04 - cantidad: 1 - precio un.: S/. 47</t>
         </is>
       </c>
-      <c r="F13" s="51" t="n">
+      <c r="F15" s="51" t="n">
         <v>47</v>
       </c>
     </row>
-    <row r="14" ht="18.75" customHeight="1">
-      <c r="A14" s="52" t="inlineStr"/>
-      <c r="E14" s="53" t="n"/>
-      <c r="F14" s="17" t="n"/>
-    </row>
-    <row r="15" ht="18.75" customHeight="1">
-      <c r="A15" s="54" t="n"/>
-      <c r="E15" s="53" t="n"/>
-      <c r="F15" s="17" t="n"/>
-    </row>
     <row r="16" ht="18.75" customFormat="1" customHeight="1" s="6">
-      <c r="A16" s="54" t="n"/>
+      <c r="A16" s="52" t="inlineStr"/>
       <c r="E16" s="53" t="n"/>
       <c r="F16" s="17" t="n"/>
     </row>
@@ -1088,132 +1098,126 @@
       <c r="F17" s="17" t="n"/>
     </row>
     <row r="18" ht="18.75" customHeight="1">
-      <c r="A18" s="55" t="n"/>
-      <c r="B18" s="56" t="n"/>
-      <c r="C18" s="56" t="n"/>
-      <c r="D18" s="56" t="n"/>
-      <c r="E18" s="57" t="n"/>
-      <c r="F18" s="18" t="n"/>
+      <c r="A18" s="54" t="n"/>
+      <c r="E18" s="53" t="n"/>
+      <c r="F18" s="17" t="n"/>
     </row>
     <row r="19" ht="18.75" customHeight="1">
-      <c r="A19" s="39" t="n"/>
-      <c r="B19" s="58" t="n"/>
-      <c r="C19" s="58" t="n"/>
-      <c r="D19" s="21" t="inlineStr">
+      <c r="A19" s="54" t="n"/>
+      <c r="E19" s="53" t="n"/>
+      <c r="F19" s="17" t="n"/>
+    </row>
+    <row r="20" ht="18.75" customHeight="1">
+      <c r="A20" s="55" t="n"/>
+      <c r="B20" s="56" t="n"/>
+      <c r="C20" s="56" t="n"/>
+      <c r="D20" s="56" t="n"/>
+      <c r="E20" s="57" t="n"/>
+      <c r="F20" s="18" t="n"/>
+    </row>
+    <row r="21" ht="18.75" customHeight="1" thickBot="1">
+      <c r="A21" s="39" t="n"/>
+      <c r="B21" s="58" t="n"/>
+      <c r="C21" s="58" t="n"/>
+      <c r="D21" s="21" t="inlineStr">
         <is>
           <t>[42]</t>
         </is>
       </c>
-      <c r="E19" s="19" t="inlineStr">
+      <c r="E21" s="19" t="inlineStr">
         <is>
           <t>SUBTOTAL</t>
         </is>
       </c>
-      <c r="F19" s="4" t="n">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="20" ht="18.75" customHeight="1">
-      <c r="A20" s="38" t="inlineStr">
+      <c r="F21" s="4" t="n">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="22" ht="18.75" customHeight="1">
+      <c r="A22" s="38" t="inlineStr">
         <is>
           <t>COMENTARIOS</t>
-        </is>
-      </c>
-      <c r="B20" s="58" t="n"/>
-      <c r="C20" s="59" t="n"/>
-      <c r="D20" s="43" t="n"/>
-      <c r="E20" s="19" t="inlineStr">
-        <is>
-          <t>TASA DE IMPUESTO</t>
-        </is>
-      </c>
-      <c r="F20" s="20" t="n">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="21" ht="18.75" customHeight="1" thickBot="1">
-      <c r="A21" s="30" t="inlineStr">
-        <is>
-          <t>1. Total a pagar en 30 días</t>
-        </is>
-      </c>
-      <c r="B21" s="58" t="n"/>
-      <c r="C21" s="59" t="n"/>
-      <c r="D21" s="43" t="n"/>
-      <c r="E21" s="19" t="inlineStr">
-        <is>
-          <t>IMPUESTO</t>
-        </is>
-      </c>
-      <c r="F21" s="4" t="n">
-        <v>8.460000000000001</v>
-      </c>
-    </row>
-    <row r="22" ht="18.75" customHeight="1">
-      <c r="A22" s="30" t="inlineStr">
-        <is>
-          <t>2. Incluya por favor el número de factura en su cheque</t>
         </is>
       </c>
       <c r="B22" s="58" t="n"/>
       <c r="C22" s="59" t="n"/>
       <c r="D22" s="43" t="n"/>
-      <c r="E22" s="24" t="inlineStr">
+      <c r="E22" s="19" t="inlineStr">
+        <is>
+          <t>TASA DE IMPUESTO</t>
+        </is>
+      </c>
+      <c r="F22" s="20" t="n">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="23" ht="18.75" customHeight="1">
+      <c r="A23" s="30" t="inlineStr">
+        <is>
+          <t>1. Total a pagar en 30 días</t>
+        </is>
+      </c>
+      <c r="B23" s="58" t="n"/>
+      <c r="C23" s="59" t="n"/>
+      <c r="D23" s="43" t="n"/>
+      <c r="E23" s="19" t="inlineStr">
+        <is>
+          <t>IMPUESTO</t>
+        </is>
+      </c>
+      <c r="F23" s="4" t="n">
+        <v>31.14</v>
+      </c>
+    </row>
+    <row r="24" ht="18.75" customHeight="1">
+      <c r="A24" s="30" t="inlineStr">
+        <is>
+          <t>2. Incluya por favor el número de factura en su cheque</t>
+        </is>
+      </c>
+      <c r="B24" s="58" t="n"/>
+      <c r="C24" s="59" t="n"/>
+      <c r="D24" s="43" t="n"/>
+      <c r="E24" s="24" t="inlineStr">
         <is>
           <t>OTRO</t>
         </is>
       </c>
-      <c r="F22" s="25" t="inlineStr">
+      <c r="F24" s="25" t="inlineStr">
         <is>
           <t>-</t>
         </is>
       </c>
-    </row>
-    <row r="23" ht="18.75" customHeight="1">
-      <c r="A23" s="27" t="n"/>
-      <c r="B23" s="27" t="n"/>
-      <c r="C23" s="27" t="n"/>
-      <c r="D23" s="43" t="n"/>
-      <c r="E23" s="22" t="inlineStr">
-        <is>
-          <t>TOTAL</t>
-        </is>
-      </c>
-      <c r="F23" s="23" t="n">
-        <v>55.46</v>
-      </c>
-    </row>
-    <row r="24" ht="18.75" customHeight="1">
-      <c r="A24" s="27" t="n"/>
-      <c r="B24" s="27" t="n"/>
-      <c r="C24" s="27" t="n"/>
-      <c r="D24" s="6" t="n"/>
-      <c r="E24" s="6" t="n"/>
-      <c r="F24" s="5" t="n"/>
     </row>
     <row r="25" ht="18.75" customHeight="1">
       <c r="A25" s="27" t="n"/>
       <c r="B25" s="27" t="n"/>
       <c r="C25" s="27" t="n"/>
-      <c r="D25" s="27" t="n"/>
-      <c r="E25" s="27" t="n"/>
-      <c r="F25" s="27" t="n"/>
+      <c r="D25" s="43" t="n"/>
+      <c r="E25" s="22" t="inlineStr">
+        <is>
+          <t>TOTAL</t>
+        </is>
+      </c>
+      <c r="F25" s="23" t="n">
+        <v>204.14</v>
+      </c>
     </row>
     <row r="26" ht="18.75" customHeight="1">
       <c r="A26" s="27" t="n"/>
       <c r="B26" s="27" t="n"/>
       <c r="C26" s="27" t="n"/>
-      <c r="D26" s="27" t="n"/>
-      <c r="E26" s="27" t="n"/>
-      <c r="F26" s="27" t="n"/>
+      <c r="D26" s="6" t="n"/>
+      <c r="E26" s="6" t="n"/>
+      <c r="F26" s="5" t="n"/>
     </row>
     <row r="27" ht="18.75" customHeight="1">
       <c r="A27" s="27" t="n"/>
       <c r="B27" s="27" t="n"/>
       <c r="C27" s="27" t="n"/>
-      <c r="D27" s="28" t="n"/>
-      <c r="E27" s="28" t="n"/>
-      <c r="F27" s="29" t="n"/>
+      <c r="D27" s="27" t="n"/>
+      <c r="E27" s="27" t="n"/>
+      <c r="F27" s="27" t="n"/>
     </row>
     <row r="28" ht="18.75" customHeight="1">
       <c r="A28" s="27" t="n"/>
@@ -1227,43 +1231,49 @@
       <c r="A29" s="27" t="n"/>
       <c r="B29" s="27" t="n"/>
       <c r="C29" s="27" t="n"/>
-      <c r="D29" s="43" t="n"/>
-      <c r="E29" s="43" t="n"/>
-      <c r="F29" s="5" t="n"/>
+      <c r="D29" s="28" t="n"/>
+      <c r="E29" s="28" t="n"/>
+      <c r="F29" s="29" t="n"/>
     </row>
     <row r="30">
       <c r="A30" s="27" t="n"/>
       <c r="B30" s="27" t="n"/>
       <c r="C30" s="27" t="n"/>
-      <c r="D30" s="28" t="n"/>
-      <c r="E30" s="28" t="n"/>
-      <c r="F30" s="29" t="n"/>
+      <c r="D30" s="27" t="n"/>
+      <c r="E30" s="27" t="n"/>
+      <c r="F30" s="27" t="n"/>
     </row>
     <row r="31">
       <c r="A31" s="27" t="n"/>
       <c r="B31" s="27" t="n"/>
       <c r="C31" s="27" t="n"/>
-      <c r="D31" s="6" t="n"/>
-      <c r="E31" s="6" t="n"/>
-      <c r="F31" s="26" t="n"/>
+      <c r="D31" s="43" t="n"/>
+      <c r="E31" s="43" t="n"/>
+      <c r="F31" s="5" t="n"/>
     </row>
     <row r="32">
       <c r="A32" s="27" t="n"/>
       <c r="B32" s="27" t="n"/>
       <c r="C32" s="27" t="n"/>
-      <c r="D32" s="6" t="n"/>
-      <c r="E32" s="6" t="n"/>
-      <c r="F32" s="26" t="n"/>
+      <c r="D32" s="28" t="n"/>
+      <c r="E32" s="28" t="n"/>
+      <c r="F32" s="29" t="n"/>
     </row>
     <row r="33">
       <c r="A33" s="27" t="n"/>
       <c r="B33" s="27" t="n"/>
       <c r="C33" s="27" t="n"/>
+      <c r="D33" s="6" t="n"/>
+      <c r="E33" s="6" t="n"/>
+      <c r="F33" s="26" t="n"/>
     </row>
     <row r="34">
       <c r="A34" s="27" t="n"/>
       <c r="B34" s="27" t="n"/>
       <c r="C34" s="27" t="n"/>
+      <c r="D34" s="6" t="n"/>
+      <c r="E34" s="6" t="n"/>
+      <c r="F34" s="26" t="n"/>
     </row>
     <row r="35">
       <c r="A35" s="27" t="n"/>
@@ -1404,6 +1414,16 @@
       <c r="A62" s="27" t="n"/>
       <c r="B62" s="27" t="n"/>
       <c r="C62" s="27" t="n"/>
+    </row>
+    <row r="63">
+      <c r="A63" s="27" t="n"/>
+      <c r="B63" s="27" t="n"/>
+      <c r="C63" s="27" t="n"/>
+    </row>
+    <row r="64">
+      <c r="A64" s="27" t="n"/>
+      <c r="B64" s="27" t="n"/>
+      <c r="C64" s="27" t="n"/>
     </row>
   </sheetData>
   <mergeCells count="13">

</xml_diff>

<commit_message>
Remove nocache decorator from inicio route and update user validation regex to allow spaces; enhance UI elements in cuentas2.html
</commit_message>
<xml_diff>
--- a/app/static/PDF/factura2_copia.xlsx
+++ b/app/static/PDF/factura2_copia.xlsx
@@ -962,7 +962,7 @@
       </c>
       <c r="F3" s="14" t="inlineStr">
         <is>
-          <t>B100-00000017</t>
+          <t>B100-00000018</t>
         </is>
       </c>
     </row>
@@ -982,7 +982,7 @@
       </c>
       <c r="F4" s="16" t="inlineStr">
         <is>
-          <t>73747576</t>
+          <t>10524578961</t>
         </is>
       </c>
     </row>
@@ -1028,7 +1028,7 @@
     <row r="9" ht="18.75" customHeight="1">
       <c r="A9" s="10" t="inlineStr">
         <is>
-          <t>Ruben Meladoblas</t>
+          <t>Empresa VALDOS I.R.L</t>
         </is>
       </c>
       <c r="F9" s="5" t="n"/>

</xml_diff>